<commit_message>
Improved update_coverage method with numpy_array masking instead of loop iteration.
</commit_message>
<xml_diff>
--- a/Optimization_Data.xlsx
+++ b/Optimization_Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mkulshre/Desktop/Drone Optimization/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C669F6E3-6AF2-8B49-9939-5B40D05D3717}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57381D64-B172-2A4B-8F61-F086D8AFCF6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="800" yWindow="2720" windowWidth="28040" windowHeight="15660" activeTab="1" xr2:uid="{E3068A53-4E07-4941-B6A0-947279A36580}"/>
+    <workbookView xWindow="760" yWindow="8680" windowWidth="28040" windowHeight="15660" xr2:uid="{E3068A53-4E07-4941-B6A0-947279A36580}"/>
   </bookViews>
   <sheets>
     <sheet name="Optimization" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="14">
   <si>
     <t>Control (no optimization)</t>
   </si>
@@ -126,6 +126,9 @@
   </si>
   <si>
     <t>Measuring generation 0 average ftiness</t>
+  </si>
+  <si>
+    <t>Numpy Array Masking</t>
   </si>
 </sst>
 </file>
@@ -254,7 +257,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -273,9 +276,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -297,7 +297,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -641,49 +641,56 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFF9084C-F84B-4D40-BFF7-E4B96BF213C9}">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="22.83203125" customWidth="1"/>
     <col min="2" max="2" width="29" customWidth="1"/>
+    <col min="3" max="3" width="28.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:3">
       <c r="B1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:2">
+      <c r="C1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:2">
+      <c r="C2" s="5">
+        <v>76.261159625020795</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:3">
       <c r="A5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:3">
       <c r="A6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:3">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -697,25 +704,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7F1AAF9-346A-D544-BED4-95E1422D43C9}">
   <dimension ref="A1:F19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="22.83203125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="36.33203125" style="13" customWidth="1"/>
-    <col min="3" max="3" width="39.33203125" style="13" customWidth="1"/>
-    <col min="4" max="5" width="10.83203125" style="14"/>
-    <col min="6" max="16384" width="10.83203125" style="15"/>
+    <col min="2" max="2" width="36.33203125" style="12" customWidth="1"/>
+    <col min="3" max="3" width="39.33203125" style="12" customWidth="1"/>
+    <col min="4" max="5" width="10.83203125" style="13"/>
+    <col min="6" max="16384" width="10.83203125" style="14"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" customFormat="1" ht="34">
       <c r="A1" s="7"/>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="9" t="s">
         <v>10</v>
       </c>
       <c r="D1" s="3"/>
@@ -723,10 +730,10 @@
       <c r="F1" s="4"/>
     </row>
     <row r="2" spans="1:6" ht="17">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="13">
+      <c r="B2" s="12">
         <v>2.47515451039374</v>
       </c>
       <c r="C2" s="5">
@@ -734,21 +741,21 @@
       </c>
     </row>
     <row r="3" spans="1:6" ht="17">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="13">
+      <c r="B3" s="12">
         <v>2.5669851334664799</v>
       </c>
-      <c r="C3" s="13">
+      <c r="C3" s="12">
         <v>2.6258057123599898</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="17">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="11">
+      <c r="B4" s="10">
         <v>2.6421564348564899</v>
       </c>
       <c r="C4" s="5">
@@ -756,10 +763,10 @@
       </c>
     </row>
     <row r="5" spans="1:6" ht="17">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="12">
+      <c r="B5" s="11">
         <v>2.3008675201492301</v>
       </c>
       <c r="C5" s="5">
@@ -767,7 +774,7 @@
       </c>
     </row>
     <row r="6" spans="1:6" ht="17">
-      <c r="A6" s="8" t="s">
+      <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="5">
@@ -777,20 +784,20 @@
         <v>2.5583361158337299</v>
       </c>
     </row>
-    <row r="7" spans="1:6" s="21" customFormat="1" ht="17">
-      <c r="A7" s="18" t="s">
+    <row r="7" spans="1:6" s="20" customFormat="1" ht="17">
+      <c r="A7" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="19">
+      <c r="B7" s="18">
         <f xml:space="preserve"> SUM(B2:B6)/5</f>
         <v>2.5039877608360817</v>
       </c>
-      <c r="C7" s="19">
+      <c r="C7" s="18">
         <f>SUM(C2:C6)/5</f>
         <v>2.5498412817080278</v>
       </c>
-      <c r="D7" s="20"/>
-      <c r="E7" s="20"/>
+      <c r="D7" s="19"/>
+      <c r="E7" s="19"/>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="2"/>
@@ -802,14 +809,14 @@
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="7"/>
-      <c r="B11" s="16"/>
-      <c r="C11" s="17"/>
+      <c r="B11" s="15"/>
+      <c r="C11" s="16"/>
     </row>
     <row r="12" spans="1:6" ht="17">
-      <c r="A12" s="8" t="s">
+      <c r="A12" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B12" s="11">
+      <c r="B12" s="10">
         <v>6.8072894901600298</v>
       </c>
       <c r="C12" s="5">
@@ -817,10 +824,10 @@
       </c>
     </row>
     <row r="13" spans="1:6" ht="17">
-      <c r="A13" s="8" t="s">
+      <c r="A13" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B13" s="11">
+      <c r="B13" s="10">
         <v>6.2126016127745496</v>
       </c>
       <c r="C13" s="5">
@@ -828,10 +835,10 @@
       </c>
     </row>
     <row r="14" spans="1:6" ht="17">
-      <c r="A14" s="8" t="s">
+      <c r="A14" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B14" s="11">
+      <c r="B14" s="10">
         <v>5.0062700196242904</v>
       </c>
       <c r="C14" s="5">
@@ -839,10 +846,10 @@
       </c>
     </row>
     <row r="15" spans="1:6" ht="17">
-      <c r="A15" s="8" t="s">
+      <c r="A15" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B15" s="12">
+      <c r="B15" s="11">
         <v>4.7008346562794596</v>
       </c>
       <c r="C15" s="5">
@@ -850,7 +857,7 @@
       </c>
     </row>
     <row r="16" spans="1:6" ht="17">
-      <c r="A16" s="8" t="s">
+      <c r="A16" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B16" s="5">
@@ -860,20 +867,20 @@
         <v>5.8342156831945999</v>
       </c>
     </row>
-    <row r="17" spans="1:5" s="21" customFormat="1" ht="17">
-      <c r="A17" s="18" t="s">
+    <row r="17" spans="1:5" s="20" customFormat="1" ht="17">
+      <c r="A17" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="B17" s="19">
+      <c r="B17" s="18">
         <f xml:space="preserve"> SUM(B12:B16)/5</f>
         <v>5.5820081737049021</v>
       </c>
-      <c r="C17" s="19">
+      <c r="C17" s="18">
         <f>SUM(C12:C16)/5</f>
         <v>6.0035840956297974</v>
       </c>
-      <c r="D17" s="20"/>
-      <c r="E17" s="20"/>
+      <c r="D17" s="19"/>
+      <c r="E17" s="19"/>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="2"/>

</xml_diff>